<commit_message>
updated stats and code to export to altair
</commit_message>
<xml_diff>
--- a/output/extra_stats.xlsx
+++ b/output/extra_stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>max_rank</t>
   </si>
@@ -68,6 +68,27 @@
   </si>
   <si>
     <t>M2_12 Wild Hunt 2020</t>
+  </si>
+  <si>
+    <t>M3_01 Wolf 2021</t>
+  </si>
+  <si>
+    <t>M3_02 Love 2021</t>
+  </si>
+  <si>
+    <t>M3_03 Bear 2021</t>
+  </si>
+  <si>
+    <t>M3_04 Elf 2021</t>
+  </si>
+  <si>
+    <t>M3_05 Viper 2021</t>
+  </si>
+  <si>
+    <t>M3_06 Magic 2021</t>
+  </si>
+  <si>
+    <t>M3_07 Griffin 2021</t>
   </si>
 </sst>
 </file>
@@ -425,7 +446,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -691,6 +712,146 @@
         <v>0.2849002849002849</v>
       </c>
     </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>13428</v>
+      </c>
+      <c r="C14">
+        <v>96</v>
+      </c>
+      <c r="D14">
+        <v>3.723562704795949</v>
+      </c>
+      <c r="E14">
+        <v>1.489425081918379</v>
+      </c>
+      <c r="F14">
+        <v>0.4766160262138814</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>16016</v>
+      </c>
+      <c r="C15">
+        <v>96</v>
+      </c>
+      <c r="D15">
+        <v>3.121878121878122</v>
+      </c>
+      <c r="E15">
+        <v>1.248751248751249</v>
+      </c>
+      <c r="F15">
+        <v>0.3996003996003996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>13636</v>
+      </c>
+      <c r="C16">
+        <v>192</v>
+      </c>
+      <c r="D16">
+        <v>3.666764447051921</v>
+      </c>
+      <c r="E16">
+        <v>1.466705778820768</v>
+      </c>
+      <c r="F16">
+        <v>0.4693458492226459</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>16049</v>
+      </c>
+      <c r="C17">
+        <v>96</v>
+      </c>
+      <c r="D17">
+        <v>3.115458907097016</v>
+      </c>
+      <c r="E17">
+        <v>1.246183562838806</v>
+      </c>
+      <c r="F17">
+        <v>0.398778740108418</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>17623</v>
+      </c>
+      <c r="C18">
+        <v>579</v>
+      </c>
+      <c r="D18">
+        <v>2.837201384554276</v>
+      </c>
+      <c r="E18">
+        <v>1.13488055382171</v>
+      </c>
+      <c r="F18">
+        <v>0.3631617772229473</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>17442</v>
+      </c>
+      <c r="C19">
+        <v>96</v>
+      </c>
+      <c r="D19">
+        <v>2.866643733516799</v>
+      </c>
+      <c r="E19">
+        <v>1.14665749340672</v>
+      </c>
+      <c r="F19">
+        <v>0.3669303978901502</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>16772</v>
+      </c>
+      <c r="C20">
+        <v>96</v>
+      </c>
+      <c r="D20">
+        <v>2.981159074648223</v>
+      </c>
+      <c r="E20">
+        <v>1.192463629859289</v>
+      </c>
+      <c r="F20">
+        <v>0.3815883615549726</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>